<commit_message>
update model, add 4-13 results, add readme
</commit_message>
<xml_diff>
--- a/IE_Scheduling Parameters.xlsx
+++ b/IE_Scheduling Parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jblak\My Drive\UARK Spring 2023\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jblak\Documents\IE_Course_Scheduling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A5F8C39-0298-4868-898B-523CB6B3A7F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C3D71FE-C0AC-4DDB-8C3D-2A6F335AE0C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="4" xr2:uid="{76F9D558-28C5-1B4A-8614-FE8704DF82C2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{76F9D558-28C5-1B4A-8614-FE8704DF82C2}"/>
   </bookViews>
   <sheets>
     <sheet name="a" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="c" sheetId="4" r:id="rId4"/>
     <sheet name="w" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1611,7 +1611,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:I23"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3944,7 +3944,7 @@
   <dimension ref="A1:W23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5593,7 +5593,7 @@
   <dimension ref="A1:O14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5659,23 +5659,23 @@
       </c>
       <c r="C2">
         <f t="shared" ref="C2:O2" ca="1" si="0">IF(RAND()&gt; 0.45,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H2">
         <f t="shared" ca="1" si="0"/>
@@ -5695,7 +5695,7 @@
       </c>
       <c r="L2">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M2">
         <f t="shared" ca="1" si="0"/>
@@ -5707,7 +5707,7 @@
       </c>
       <c r="O2">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -5720,7 +5720,7 @@
       </c>
       <c r="C3">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3">
         <f t="shared" ca="1" si="1"/>
@@ -5728,7 +5728,7 @@
       </c>
       <c r="E3">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3">
         <f t="shared" ca="1" si="1"/>
@@ -5736,11 +5736,11 @@
       </c>
       <c r="G3">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H3">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I3">
         <f t="shared" ca="1" si="1"/>
@@ -5748,15 +5748,15 @@
       </c>
       <c r="J3">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K3">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L3">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M3">
         <f t="shared" ca="1" si="1"/>
@@ -5777,23 +5777,23 @@
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="1"/>
@@ -5805,7 +5805,7 @@
       </c>
       <c r="I4">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J4">
         <f t="shared" ca="1" si="1"/>
@@ -5829,7 +5829,7 @@
       </c>
       <c r="O4">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -5838,11 +5838,11 @@
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="1"/>
@@ -5866,11 +5866,11 @@
       </c>
       <c r="I5">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K5">
         <f t="shared" ca="1" si="1"/>
@@ -5878,19 +5878,19 @@
       </c>
       <c r="L5">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M5">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N5">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O5">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -5899,7 +5899,7 @@
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="1"/>
@@ -5911,7 +5911,7 @@
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="1"/>
@@ -5923,7 +5923,7 @@
       </c>
       <c r="H6">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6">
         <f t="shared" ca="1" si="1"/>
@@ -5939,7 +5939,7 @@
       </c>
       <c r="L6">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M6">
         <f t="shared" ca="1" si="1"/>
@@ -5951,7 +5951,7 @@
       </c>
       <c r="O6">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5960,15 +5960,15 @@
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="1"/>
@@ -5976,7 +5976,7 @@
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G7">
         <f t="shared" ca="1" si="1"/>
@@ -5984,7 +5984,7 @@
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7">
         <f t="shared" ca="1" si="1"/>
@@ -5992,11 +5992,11 @@
       </c>
       <c r="J7">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K7">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L7">
         <f t="shared" ca="1" si="1"/>
@@ -6033,7 +6033,7 @@
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="1"/>
@@ -6045,23 +6045,23 @@
       </c>
       <c r="H8">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I8">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J8">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K8">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L8">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M8">
         <f t="shared" ca="1" si="1"/>
@@ -6069,7 +6069,7 @@
       </c>
       <c r="N8">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O8">
         <f t="shared" ca="1" si="1"/>
@@ -6086,11 +6086,11 @@
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="1"/>
@@ -6106,15 +6106,15 @@
       </c>
       <c r="H9">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I9">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J9">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K9">
         <f t="shared" ca="1" si="1"/>
@@ -6134,7 +6134,7 @@
       </c>
       <c r="O9">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -6143,11 +6143,11 @@
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="1"/>
@@ -6179,11 +6179,11 @@
       </c>
       <c r="K10">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L10">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M10">
         <f t="shared" ca="1" si="1"/>
@@ -6191,7 +6191,7 @@
       </c>
       <c r="N10">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O10">
         <f t="shared" ca="1" si="1"/>
@@ -6204,7 +6204,7 @@
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="1"/>
@@ -6216,11 +6216,11 @@
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11">
         <f t="shared" ca="1" si="1"/>
@@ -6248,7 +6248,7 @@
       </c>
       <c r="M11">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N11">
         <f t="shared" ca="1" si="1"/>
@@ -6269,7 +6269,7 @@
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="1"/>
@@ -6277,7 +6277,7 @@
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12">
         <f t="shared" ca="1" si="1"/>
@@ -6297,19 +6297,19 @@
       </c>
       <c r="J12">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K12">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L12">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M12">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N12">
         <f t="shared" ca="1" si="1"/>
@@ -6317,7 +6317,7 @@
       </c>
       <c r="O12">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -6334,7 +6334,7 @@
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="1"/>
@@ -6346,11 +6346,11 @@
       </c>
       <c r="G13">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H13">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I13">
         <f t="shared" ca="1" si="1"/>
@@ -6370,11 +6370,11 @@
       </c>
       <c r="M13">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N13">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O13">
         <f t="shared" ca="1" si="1"/>
@@ -6391,7 +6391,7 @@
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="1"/>
@@ -6399,11 +6399,11 @@
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G14">
         <f t="shared" ca="1" si="1"/>
@@ -6419,11 +6419,11 @@
       </c>
       <c r="J14">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K14">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L14">
         <f t="shared" ca="1" si="1"/>
@@ -6431,11 +6431,11 @@
       </c>
       <c r="M14">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N14">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O14">
         <f t="shared" ca="1" si="1"/>

</xml_diff>

<commit_message>
update md output and create resultsets
</commit_message>
<xml_diff>
--- a/IE_Scheduling Parameters.xlsx
+++ b/IE_Scheduling Parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jblak\Documents\IE_Course_Scheduling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C3D71FE-C0AC-4DDB-8C3D-2A6F335AE0C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0FBCB1A-A72D-406C-855C-FDB81DD63924}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{76F9D558-28C5-1B4A-8614-FE8704DF82C2}"/>
+    <workbookView xWindow="3315" yWindow="1995" windowWidth="28770" windowHeight="15450" activeTab="4" xr2:uid="{76F9D558-28C5-1B4A-8614-FE8704DF82C2}"/>
   </bookViews>
   <sheets>
     <sheet name="a" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="39">
   <si>
     <t>Crisel</t>
   </si>
@@ -154,6 +154,9 @@
   </si>
   <si>
     <t>Instructor</t>
+  </si>
+  <si>
+    <t>% unavail</t>
   </si>
 </sst>
 </file>
@@ -5590,10 +5593,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1E37A25-7A2F-42D0-AF79-23A530E5CE08}">
-  <dimension ref="A1:O14"/>
+  <dimension ref="A1:R14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection sqref="A1:O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5602,7 +5605,7 @@
     <col min="5" max="5" width="10.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>35</v>
       </c>
@@ -5649,16 +5652,16 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>23</v>
       </c>
       <c r="B2">
-        <f ca="1">IF(RAND()&gt; 0.45,1,0)</f>
-        <v>0</v>
+        <f ca="1">IF(RAND()&gt; $R$2,1,0)</f>
+        <v>1</v>
       </c>
       <c r="C2">
-        <f t="shared" ref="C2:O2" ca="1" si="0">IF(RAND()&gt; 0.45,1,0)</f>
+        <f t="shared" ref="C2:O2" ca="1" si="0">IF(RAND()&gt; $R$2,1,0)</f>
         <v>0</v>
       </c>
       <c r="D2">
@@ -5683,15 +5686,15 @@
       </c>
       <c r="I2">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J2">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K2">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L2">
         <f t="shared" ca="1" si="0"/>
@@ -5699,24 +5702,30 @@
       </c>
       <c r="M2">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N2">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O2">
         <f t="shared" ca="1" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q2" t="s">
+        <v>38</v>
+      </c>
+      <c r="R2">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:O14" ca="1" si="1">IF(RAND()&gt; 0.45,1,0)</f>
-        <v>0</v>
+        <f t="shared" ref="B3:O14" ca="1" si="1">IF(RAND()&gt; $R$2,1,0)</f>
+        <v>1</v>
       </c>
       <c r="C3">
         <f t="shared" ca="1" si="1"/>
@@ -5728,27 +5737,27 @@
       </c>
       <c r="E3">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H3">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I3">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J3">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K3">
         <f t="shared" ca="1" si="1"/>
@@ -5756,7 +5765,7 @@
       </c>
       <c r="L3">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M3">
         <f t="shared" ca="1" si="1"/>
@@ -5764,14 +5773,14 @@
       </c>
       <c r="N3">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O3">
         <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -5793,7 +5802,7 @@
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="1"/>
@@ -5801,15 +5810,15 @@
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I4">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J4">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K4">
         <f t="shared" ca="1" si="1"/>
@@ -5825,14 +5834,14 @@
       </c>
       <c r="N4">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O4">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -5842,15 +5851,15 @@
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="1"/>
@@ -5862,7 +5871,7 @@
       </c>
       <c r="H5">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5">
         <f t="shared" ca="1" si="1"/>
@@ -5878,7 +5887,7 @@
       </c>
       <c r="L5">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M5">
         <f t="shared" ca="1" si="1"/>
@@ -5890,10 +5899,10 @@
       </c>
       <c r="O5">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -5935,11 +5944,11 @@
       </c>
       <c r="K6">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L6">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M6">
         <f t="shared" ca="1" si="1"/>
@@ -5947,28 +5956,28 @@
       </c>
       <c r="N6">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O6">
         <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>27</v>
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="1"/>
@@ -5976,7 +5985,7 @@
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7">
         <f t="shared" ca="1" si="1"/>
@@ -5988,7 +5997,7 @@
       </c>
       <c r="I7">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7">
         <f t="shared" ca="1" si="1"/>
@@ -6004,24 +6013,24 @@
       </c>
       <c r="M7">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N7">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O7">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>28</v>
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="1"/>
@@ -6037,7 +6046,7 @@
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8">
         <f t="shared" ca="1" si="1"/>
@@ -6045,7 +6054,7 @@
       </c>
       <c r="H8">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8">
         <f t="shared" ca="1" si="1"/>
@@ -6057,15 +6066,15 @@
       </c>
       <c r="K8">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L8">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M8">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N8">
         <f t="shared" ca="1" si="1"/>
@@ -6073,20 +6082,20 @@
       </c>
       <c r="O8">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>29</v>
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="1"/>
@@ -6094,11 +6103,11 @@
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9">
         <f t="shared" ca="1" si="1"/>
@@ -6110,7 +6119,7 @@
       </c>
       <c r="I9">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J9">
         <f t="shared" ca="1" si="1"/>
@@ -6118,15 +6127,15 @@
       </c>
       <c r="K9">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L9">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M9">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N9">
         <f t="shared" ca="1" si="1"/>
@@ -6134,16 +6143,16 @@
       </c>
       <c r="O9">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>30</v>
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="1"/>
@@ -6171,7 +6180,7 @@
       </c>
       <c r="I10">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J10">
         <f t="shared" ca="1" si="1"/>
@@ -6187,24 +6196,24 @@
       </c>
       <c r="M10">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N10">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O10">
         <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>31</v>
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="1"/>
@@ -6232,7 +6241,7 @@
       </c>
       <c r="I11">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J11">
         <f t="shared" ca="1" si="1"/>
@@ -6244,7 +6253,7 @@
       </c>
       <c r="L11">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M11">
         <f t="shared" ca="1" si="1"/>
@@ -6252,14 +6261,14 @@
       </c>
       <c r="N11">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O11">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -6277,7 +6286,7 @@
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12">
         <f t="shared" ca="1" si="1"/>
@@ -6289,7 +6298,7 @@
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I12">
         <f t="shared" ca="1" si="1"/>
@@ -6301,7 +6310,7 @@
       </c>
       <c r="K12">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L12">
         <f t="shared" ca="1" si="1"/>
@@ -6313,14 +6322,14 @@
       </c>
       <c r="N12">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O12">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -6342,7 +6351,7 @@
       </c>
       <c r="F13">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13">
         <f t="shared" ca="1" si="1"/>
@@ -6354,7 +6363,7 @@
       </c>
       <c r="I13">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J13">
         <f t="shared" ca="1" si="1"/>
@@ -6374,14 +6383,14 @@
       </c>
       <c r="N13">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O13">
         <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>34</v>
       </c>
@@ -6391,11 +6400,11 @@
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="1"/>
@@ -6403,7 +6412,7 @@
       </c>
       <c r="F14">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14">
         <f t="shared" ca="1" si="1"/>
@@ -6415,11 +6424,11 @@
       </c>
       <c r="I14">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K14">
         <f t="shared" ca="1" si="1"/>

</xml_diff>